<commit_message>
Task work somehow. but still TBU
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -20,15 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
-  <si>
-    <t xml:space="preserve">Меню</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+  <si>
+    <t xml:space="preserve">ыпывап</t>
   </si>
   <si>
     <t xml:space="preserve">Основное меню</t>
   </si>
   <si>
-    <t xml:space="preserve">Холодные закуски</t>
+    <t xml:space="preserve">пывап</t>
   </si>
   <si>
     <t xml:space="preserve">К пиву</t>
@@ -46,12 +46,18 @@
     <t xml:space="preserve">Нарезка из ветчины, колбасных колечек, нескольких сортов сыра и фруктов</t>
   </si>
   <si>
-    <t xml:space="preserve">Рыбная тарелка</t>
+    <t xml:space="preserve">авпыавп</t>
   </si>
   <si>
     <t xml:space="preserve">Нарезка из креветок, кальмаров, раковых шеек, гребешков, лосося, скумбрии и красной икры</t>
   </si>
   <si>
+    <t xml:space="preserve">выапфып</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ыфпфвып</t>
+  </si>
+  <si>
     <t xml:space="preserve">Рамен</t>
   </si>
   <si>
@@ -128,6 +134,27 @@
   </si>
   <si>
     <t xml:space="preserve">Это купаж высококачественных солодовых и зерновых виски, выдержанных как минимум в течение 12 лет, что придает напитку роскошные нотки меда, ванили и спелых яблок.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ыва</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ывп</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ываыва</t>
+  </si>
+  <si>
+    <t xml:space="preserve">фпфвып</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ватвртвп</t>
+  </si>
+  <si>
+    <t xml:space="preserve">фывафыв</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ваптвпат</t>
   </si>
 </sst>
 </file>
@@ -271,10 +298,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:F1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -284,7 +311,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="21.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="77.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -365,39 +392,39 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
-      <c r="B6" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="3"/>
+      <c r="F6" s="3" t="n">
+        <v>265.57</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3" t="n">
-        <v>1</v>
+      <c r="B7" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="3" t="n">
-        <v>166.47</v>
-      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>14</v>
@@ -406,14 +433,14 @@
         <v>15</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>168.25</v>
+        <v>166.47</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>16</v>
@@ -422,58 +449,58 @@
         <v>17</v>
       </c>
       <c r="F9" s="3" t="n">
+        <v>168.25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="3" t="n">
         <v>132.88</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3" t="n">
-        <v>1</v>
+      <c r="B11" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="D11" s="4"/>
       <c r="E11" s="6"/>
       <c r="F11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="5" t="n">
+      <c r="B12" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="D12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="3" t="n">
-        <v>2700.79</v>
-      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>24</v>
@@ -482,14 +509,14 @@
         <v>25</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>3100.33</v>
+        <v>2700.79</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>26</v>
@@ -498,44 +525,44 @@
         <v>27</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>1850.42</v>
+        <v>3100.33</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
-      <c r="B15" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="3"/>
+      <c r="C15" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="3"/>
+      <c r="F15" s="3" t="n">
+        <v>1850.42</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3" t="n">
-        <v>1</v>
+      <c r="B16" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="3" t="n">
-        <v>420.78</v>
-      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>32</v>
@@ -544,14 +571,14 @@
         <v>33</v>
       </c>
       <c r="F17" s="3" t="n">
-        <v>440.11</v>
+        <v>420.78</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>34</v>
@@ -560,15 +587,89 @@
         <v>35</v>
       </c>
       <c r="F18" s="3" t="n">
+        <v>440.11</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="3" t="n">
         <v>520.08</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B21" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C22" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>420.78</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C23" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="3" t="n">
+        <v>440.11</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C24" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="3" t="n">
+        <v>520.08</v>
+      </c>
+    </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1545,6 +1646,7 @@
     <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1001" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Task work somehow. loop issues fix
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -20,15 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
-  <si>
-    <t xml:space="preserve">ыпывап</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+  <si>
+    <t xml:space="preserve">Меню</t>
   </si>
   <si>
     <t xml:space="preserve">Основное меню</t>
   </si>
   <si>
-    <t xml:space="preserve">пывап</t>
+    <t xml:space="preserve">Холодные закуски</t>
   </si>
   <si>
     <t xml:space="preserve">К пиву</t>
@@ -46,18 +46,12 @@
     <t xml:space="preserve">Нарезка из ветчины, колбасных колечек, нескольких сортов сыра и фруктов</t>
   </si>
   <si>
-    <t xml:space="preserve">авпыавп</t>
+    <t xml:space="preserve">Рыбная тарелка</t>
   </si>
   <si>
     <t xml:space="preserve">Нарезка из креветок, кальмаров, раковых шеек, гребешков, лосося, скумбрии и красной икры</t>
   </si>
   <si>
-    <t xml:space="preserve">выапфып</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ыфпфвып</t>
-  </si>
-  <si>
     <t xml:space="preserve">Рамен</t>
   </si>
   <si>
@@ -134,27 +128,6 @@
   </si>
   <si>
     <t xml:space="preserve">Это купаж высококачественных солодовых и зерновых виски, выдержанных как минимум в течение 12 лет, что придает напитку роскошные нотки меда, ванили и спелых яблок.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ыва</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ывп</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ываыва</t>
-  </si>
-  <si>
-    <t xml:space="preserve">фпфвып</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ватвртвп</t>
-  </si>
-  <si>
-    <t xml:space="preserve">фывафыв</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ваптвпат</t>
   </si>
 </sst>
 </file>
@@ -248,12 +221,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -301,375 +270,301 @@
   <dimension ref="A1:F1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="77.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="77.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="n">
+      <c r="A1" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3" t="n">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="5" t="n">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="2" t="n">
         <v>182.99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="5" t="n">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="2" t="n">
         <v>215.36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="5" t="n">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="2" t="n">
         <v>265.57</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="D6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="3" t="n">
-        <v>265.57</v>
-      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3" t="n">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>166.47</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3" t="n">
+      <c r="D8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>168.25</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>132.88</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="3" t="n">
-        <v>166.47</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3" t="n">
+      <c r="C11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>2700.79</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="3" t="n">
-        <v>168.25</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3" t="n">
+      <c r="D13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>3100.33</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="3" t="n">
-        <v>132.88</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+      <c r="D14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>1850.42</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3" t="n">
+      <c r="C15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="3" t="n">
-        <v>2700.79</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="5" t="n">
+      <c r="D16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>420.78</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="3" t="n">
-        <v>3100.33</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="5" t="n">
+      <c r="D17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>440.11</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="3" t="n">
-        <v>1850.42</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="3" t="n">
-        <v>420.78</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="3" t="n">
-        <v>440.11</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F19" s="3" t="n">
+      <c r="F18" s="2" t="n">
         <v>520.08</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C22" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" s="3" t="n">
-        <v>420.78</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C23" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" s="3" t="n">
-        <v>440.11</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C24" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F24" s="3" t="n">
-        <v>520.08</v>
-      </c>
-    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1646,7 +1541,7 @@
     <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1001" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1001" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>